<commit_message>
Update process names and define INDELC at DAYNITE level
</commit_message>
<xml_diff>
--- a/VT_IE_IND.xlsx
+++ b/VT_IE_IND.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFECD2B6-30BE-4E0F-B41F-0DB63BB8392C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DF0226-7484-4424-A510-305BFF43AB9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="302">
   <si>
     <t>Development</t>
   </si>
@@ -10761,7 +10761,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" cellComments="asDisplayed" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="landscape" cellComments="asDisplayed" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Myriad Pro,Regular"&amp;14Ireland's Energy Balance &amp;A</oddHeader>
     <oddFooter>&amp;L&amp;G&amp;RPage &amp;P of &amp;N</oddFooter>
@@ -10774,8 +10774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1C8D34-EFD7-45C2-8418-665049CA220F}">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11035,7 +11035,9 @@
         <v>189</v>
       </c>
       <c r="G13" s="277"/>
-      <c r="H13" s="277"/>
+      <c r="H13" s="277" t="s">
+        <v>261</v>
+      </c>
       <c r="I13" s="277"/>
       <c r="J13" s="277"/>
     </row>
@@ -11660,7 +11662,7 @@
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11737,8 +11739,8 @@
         <v>IE,National</v>
       </c>
       <c r="D5" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D18,2,3))</f>
-        <v>I-DMD-NEM</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B5,MID(Commodities!D18,2,3),"E0")</f>
+        <v>I-DMD-NEM-E0</v>
       </c>
       <c r="E5" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E18," process")</f>
@@ -11763,8 +11765,8 @@
         <v>IE,National</v>
       </c>
       <c r="D6" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D19,2,3))</f>
-        <v>I-DMD-FAB</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B6,MID(Commodities!D19,2,3),"E0")</f>
+        <v>I-DMD-FAB-E0</v>
       </c>
       <c r="E6" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E19," process")</f>
@@ -11789,8 +11791,8 @@
         <v>IE,National</v>
       </c>
       <c r="D7" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D20,2,3))</f>
-        <v>I-DMD-TAP</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B7,MID(Commodities!D20,2,3),"E0")</f>
+        <v>I-DMD-TAP-E0</v>
       </c>
       <c r="E7" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E20," process")</f>
@@ -11815,8 +11817,8 @@
         <v>IE,National</v>
       </c>
       <c r="D8" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D21,2,3))</f>
-        <v>I-DMD-WAP</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B8,MID(Commodities!D21,2,3),"E0")</f>
+        <v>I-DMD-WAP-E0</v>
       </c>
       <c r="E8" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E21," process")</f>
@@ -11841,8 +11843,8 @@
         <v>IE,National</v>
       </c>
       <c r="D9" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D22,2,3))</f>
-        <v>I-DMD-PX4</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B9,MID(Commodities!D22,2,3),"E0")</f>
+        <v>I-DMD-PX4-E0</v>
       </c>
       <c r="E9" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E22," process")</f>
@@ -11867,8 +11869,8 @@
         <v>IE,National</v>
       </c>
       <c r="D10" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D23,2,3))</f>
-        <v>I-DMD-CAF</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B10,MID(Commodities!D23,2,3),"E0")</f>
+        <v>I-DMD-CAF-E0</v>
       </c>
       <c r="E10" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E23," process")</f>
@@ -11893,8 +11895,8 @@
         <v>IE,National</v>
       </c>
       <c r="D11" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D24,2,3))</f>
-        <v>I-DMD-RAP</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B11,MID(Commodities!D24,2,3),"E0")</f>
+        <v>I-DMD-RAP-E0</v>
       </c>
       <c r="E11" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E24," process")</f>
@@ -11919,8 +11921,8 @@
         <v>IE,National</v>
       </c>
       <c r="D12" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D25,2,3))</f>
-        <v>I-DMD-ONM</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B12,MID(Commodities!D25,2,3),"E0")</f>
+        <v>I-DMD-ONM-E0</v>
       </c>
       <c r="E12" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E25," process")</f>
@@ -11945,8 +11947,8 @@
         <v>IE,National</v>
       </c>
       <c r="D13" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D26,2,3))</f>
-        <v>I-DMD-MAP</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B13,MID(Commodities!D26,2,3),"E0")</f>
+        <v>I-DMD-MAP-E0</v>
       </c>
       <c r="E13" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E26," process")</f>
@@ -11971,8 +11973,8 @@
         <v>IE,National</v>
       </c>
       <c r="D14" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D27,2,3))</f>
-        <v>I-DMD-MAE</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B14,MID(Commodities!D27,2,3),"E0")</f>
+        <v>I-DMD-MAE-E0</v>
       </c>
       <c r="E14" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E27," process")</f>
@@ -11997,8 +11999,8 @@
         <v>IE,National</v>
       </c>
       <c r="D15" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D28,2,3))</f>
-        <v>I-DMD-EOE</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B15,MID(Commodities!D28,2,3),"E0")</f>
+        <v>I-DMD-EOE-E0</v>
       </c>
       <c r="E15" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E28," process")</f>
@@ -12023,8 +12025,8 @@
         <v>IE,National</v>
       </c>
       <c r="D16" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D29,2,3))</f>
-        <v>I-DMD-TEM</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B16,MID(Commodities!D29,2,3),"E0")</f>
+        <v>I-DMD-TEM-E0</v>
       </c>
       <c r="E16" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E29," process")</f>
@@ -12049,8 +12051,8 @@
         <v>IE,National</v>
       </c>
       <c r="D17" s="278" t="str">
-        <f>_xlfn.CONCAT("I-DMD-",MID(Commodities!D30,2,3))</f>
-        <v>I-DMD-OMA</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B17,MID(Commodities!D30,2,3),"E0")</f>
+        <v>I-DMD-OMA-E0</v>
       </c>
       <c r="E17" s="278" t="str">
         <f>_xlfn.CONCAT(Commodities!E30," process")</f>
@@ -12088,11 +12090,11 @@
         <v>IE,National</v>
       </c>
       <c r="D19" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D5)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D5)</f>
         <v>FT-INDCOA</v>
       </c>
       <c r="E19" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E5)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E5)</f>
         <v>Fuel Tech - Coal (IND)</v>
       </c>
       <c r="F19" s="286" t="s">
@@ -12114,11 +12116,11 @@
         <v>IE,National</v>
       </c>
       <c r="D20" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D6)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D6)</f>
         <v>FT-INDPEA</v>
       </c>
       <c r="E20" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E6)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E6)</f>
         <v xml:space="preserve">Fuel Tech - Peat (IND) </v>
       </c>
       <c r="F20" s="287" t="s">
@@ -12140,11 +12142,11 @@
         <v>IE,National</v>
       </c>
       <c r="D21" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D7)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D7)</f>
         <v>FT-INDKER</v>
       </c>
       <c r="E21" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E7)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E7)</f>
         <v>Fuel Tech - Kerosene (IND)</v>
       </c>
       <c r="F21" s="287" t="s">
@@ -12166,11 +12168,11 @@
         <v>IE,National</v>
       </c>
       <c r="D22" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D8)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D8)</f>
         <v>FT-INDHFO</v>
       </c>
       <c r="E22" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E8)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E8)</f>
         <v>Fuel Tech - Heavy Fuel Oil (IND)</v>
       </c>
       <c r="F22" s="287" t="s">
@@ -12192,11 +12194,11 @@
         <v>IE,National</v>
       </c>
       <c r="D23" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D9)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D9)</f>
         <v>FT-INDLPG</v>
       </c>
       <c r="E23" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E9)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E9)</f>
         <v>Fuel Tech - Liquified Petroleum Gas (IND)</v>
       </c>
       <c r="F23" s="287" t="s">
@@ -12218,11 +12220,11 @@
         <v>IE,National</v>
       </c>
       <c r="D24" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D10)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D10)</f>
         <v>FT-INDDST</v>
       </c>
       <c r="E24" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E10)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E10)</f>
         <v>Fuel Tech - Diesel (IND)</v>
       </c>
       <c r="F24" s="287" t="s">
@@ -12244,11 +12246,11 @@
         <v>IE,National</v>
       </c>
       <c r="D25" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D11)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D11)</f>
         <v>FT-INDCOK</v>
       </c>
       <c r="E25" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E11)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E11)</f>
         <v>Fuel Tech - Petroleum Coke (IND)</v>
       </c>
       <c r="F25" s="287" t="s">
@@ -12270,11 +12272,11 @@
         <v>IE,National</v>
       </c>
       <c r="D26" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D12)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D12)</f>
         <v>FT-INDGAS</v>
       </c>
       <c r="E26" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E12)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E12)</f>
         <v>Fuel Tech - Natural Gas (IND)</v>
       </c>
       <c r="F26" s="287" t="s">
@@ -12296,11 +12298,11 @@
         <v>IE,National</v>
       </c>
       <c r="D27" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D13)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D13)</f>
         <v>FT-INDELC</v>
       </c>
       <c r="E27" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E13)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E13)</f>
         <v>Fuel Tech - Electricity (IND)</v>
       </c>
       <c r="F27" s="287" t="s">
@@ -12324,11 +12326,11 @@
         <v>IE,National</v>
       </c>
       <c r="D28" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D14)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D14)</f>
         <v>FT-INDBGS</v>
       </c>
       <c r="E28" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E14)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E14)</f>
         <v>Fuel Tech - Biogas (IND)</v>
       </c>
       <c r="F28" s="287" t="s">
@@ -12350,11 +12352,11 @@
         <v>IE,National</v>
       </c>
       <c r="D29" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D15)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D15)</f>
         <v>FT-INDBRW</v>
       </c>
       <c r="E29" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E15)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E15)</f>
         <v>Fuel Tech - Biomass and renewable waste (IND)</v>
       </c>
       <c r="F29" s="287" t="s">
@@ -12376,11 +12378,11 @@
         <v>IE,National</v>
       </c>
       <c r="D30" s="278" t="str">
-        <f>_xlfn.CONCAT("FT-",Commodities!D16)</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D16)</f>
         <v>FT-INDNRW</v>
       </c>
       <c r="E30" s="278" t="str">
-        <f>_xlfn.CONCAT("Fuel Tech - ",Commodities!E16)</f>
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E16)</f>
         <v>Fuel Tech - Non-renewable waste (IND)</v>
       </c>
       <c r="F30" s="287" t="s">
@@ -12820,8 +12822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DF8194-EAB2-4AAC-9B35-F09487A4BBC8}">
   <dimension ref="B2:Y102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12929,7 +12931,7 @@
       </c>
       <c r="C6" s="292" t="str">
         <f>Processes!D5</f>
-        <v>I-DMD-NEM</v>
+        <v>I-DMD-NEM-E0</v>
       </c>
       <c r="D6" s="292" t="str">
         <f>Processes!E5</f>
@@ -13155,7 +13157,7 @@
       </c>
       <c r="C13" s="292" t="str">
         <f>Processes!D6</f>
-        <v>I-DMD-FAB</v>
+        <v>I-DMD-FAB-E0</v>
       </c>
       <c r="D13" s="292" t="str">
         <f>Processes!E6</f>
@@ -13354,7 +13356,7 @@
       </c>
       <c r="C23" s="292" t="str">
         <f>Processes!D7</f>
-        <v>I-DMD-TAP</v>
+        <v>I-DMD-TAP-E0</v>
       </c>
       <c r="D23" s="292" t="str">
         <f>Processes!E7</f>
@@ -13489,7 +13491,7 @@
       </c>
       <c r="C30" s="292" t="str">
         <f>Processes!D8</f>
-        <v>I-DMD-WAP</v>
+        <v>I-DMD-WAP-E0</v>
       </c>
       <c r="D30" s="292" t="str">
         <f>Processes!E8</f>
@@ -13642,7 +13644,7 @@
       </c>
       <c r="C38" s="292" t="str">
         <f>Processes!D9</f>
-        <v>I-DMD-PX4</v>
+        <v>I-DMD-PX4-E0</v>
       </c>
       <c r="D38" s="292" t="str">
         <f>Processes!E9</f>
@@ -13777,7 +13779,7 @@
       </c>
       <c r="C45" s="292" t="str">
         <f>Processes!D10</f>
-        <v>I-DMD-CAF</v>
+        <v>I-DMD-CAF-E0</v>
       </c>
       <c r="D45" s="292" t="str">
         <f>Processes!E10</f>
@@ -13912,7 +13914,7 @@
       </c>
       <c r="C52" s="292" t="str">
         <f>Processes!D11</f>
-        <v>I-DMD-RAP</v>
+        <v>I-DMD-RAP-E0</v>
       </c>
       <c r="D52" s="292" t="str">
         <f>Processes!E11</f>
@@ -14047,7 +14049,7 @@
       </c>
       <c r="C59" s="292" t="str">
         <f>Processes!D12</f>
-        <v>I-DMD-ONM</v>
+        <v>I-DMD-ONM-E0</v>
       </c>
       <c r="D59" s="292" t="str">
         <f>Processes!E12</f>
@@ -14245,7 +14247,7 @@
       </c>
       <c r="C69" s="292" t="str">
         <f>Processes!D13</f>
-        <v>I-DMD-MAP</v>
+        <v>I-DMD-MAP-E0</v>
       </c>
       <c r="D69" s="292" t="str">
         <f>Processes!E13</f>
@@ -14362,7 +14364,7 @@
       </c>
       <c r="C75" s="292" t="str">
         <f>Processes!D14</f>
-        <v>I-DMD-MAE</v>
+        <v>I-DMD-MAE-E0</v>
       </c>
       <c r="D75" s="292" t="str">
         <f>Processes!E14</f>
@@ -14497,7 +14499,7 @@
       </c>
       <c r="C82" s="292" t="str">
         <f>Processes!D15</f>
-        <v>I-DMD-EOE</v>
+        <v>I-DMD-EOE-E0</v>
       </c>
       <c r="D82" s="292" t="str">
         <f>Processes!E15</f>
@@ -14632,7 +14634,7 @@
       </c>
       <c r="C89" s="292" t="str">
         <f>Processes!D16</f>
-        <v>I-DMD-TEM</v>
+        <v>I-DMD-TEM-E0</v>
       </c>
       <c r="D89" s="292" t="str">
         <f>Processes!E16</f>
@@ -14767,7 +14769,7 @@
       </c>
       <c r="C96" s="292" t="str">
         <f>Processes!D17</f>
-        <v>I-DMD-OMA</v>
+        <v>I-DMD-OMA-E0</v>
       </c>
       <c r="D96" s="292" t="str">
         <f>Processes!E17</f>
@@ -14880,7 +14882,7 @@
   <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix issues in TRA and SUP, and remove custom styles
- remove custom styles from all the files
- don't define technologies for National in TRA
- connect TRA Hydrogen
- apply formatting in TRA similar to the rest of the model
- bring back cycling and walking in SUP
</commit_message>
<xml_diff>
--- a/VT_IE_IND.xlsx
+++ b/VT_IE_IND.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAB908F-E133-42B9-8910-F5F70F998DAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B626DC79-6082-473E-8B46-D507BD580B9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1096,14 +1096,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0;[Red]\-#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="\Te\x\t"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1118,10 +1118,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1229,17 +1225,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="MS Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Myriad Pro"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -3312,85 +3298,81 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="334">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="140" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="135" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="135" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="11" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="140" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="135" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="135" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="13" fillId="11" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3400,858 +3382,854 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="56" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="57" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="62" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="64" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="65" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="66" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="65" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="67" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="68" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="70" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="72" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="73" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="78" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="79" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="82" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="84" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="87" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="89" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="90" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="91" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="92" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="93" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="92" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="94" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="95" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="96" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="97" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="98" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="82" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="79" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="84" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="99" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="100" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="101" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="101" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="102" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="103" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="104" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="105" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="106" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="101" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="107" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="108" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="103" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="104" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="105" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="106" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="101" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="87" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="109" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="109" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="110" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="111" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="112" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="113" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="114" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="115" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="109" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="116" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="141" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="117" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="110" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="111" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="113" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="109" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="116" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="118" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="119" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="117" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="142" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="121" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="122" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="120" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="117" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="123" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="121" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="120" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="26" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="143" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="26" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="143" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="121" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="69" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="121" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="70" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="145" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="146" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="147" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="148" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="149" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="150" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="59" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="144" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="145" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="146" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="147" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="148" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="149" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="150" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="62" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="118" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="122" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="68" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="125" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="124" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="126" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="127" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="128" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="129" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="130" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="72" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="73" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="135" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="125" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="126" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="131" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="138" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="132" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="134" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="133" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="135" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="136" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="137" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="151" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="138" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="132" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="133" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="137" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="151" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="64" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="66" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="64" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="143" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="130" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="129" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="127" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="143" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="70" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="73" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="23" fillId="0" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="144" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="20" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="66" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="95" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="96" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="152" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="65" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="117" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="152" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="118" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="123" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="153" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="154" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="117" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="121" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="155" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="156" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="89" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="90" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="91" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="90" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="93" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="69" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="153" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="154" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="121" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="155" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="156" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="19" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="90" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="139" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="139" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="40" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="38" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="5" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="40" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Comma" xfId="3" builtinId="3"/>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{E8F6FC94-FE00-481A-9CCA-C8F8BD082BFB}"/>
-    <cellStyle name="Normal_1990 and 1998 CIP - Prices Quantity and CO2(MH)" xfId="5" xr:uid="{27FF5463-3C49-4F90-AD36-067F6D06AECD}"/>
-    <cellStyle name="Normal_2000balx" xfId="4" xr:uid="{AB8575F7-74D3-4160-8D89-AF3ED2CFA2FE}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{1F406535-6DD4-4D28-A28F-5561F262E64A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4596,6 +4574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55B3FAE-9396-4BDD-9414-7E1233A8EF20}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4610,13 +4589,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABF3F7C-BFBC-4340-9D7B-B6BFDABDF79E}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
@@ -4648,7 +4628,7 @@
     <col min="31" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15">
+    <row r="3" spans="1:30">
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -4767,7 +4747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4882,7 +4862,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4999,7 +4979,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5332,7 +5312,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15">
+    <row r="37" spans="1:2">
       <c r="A37" s="7" t="s">
         <v>59</v>
       </c>
@@ -5375,7 +5355,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6617C6-BD81-4C8E-89D7-FC0076ADEEA7}">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AS81"/>
@@ -12708,6 +12688,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1C8D34-EFD7-45C2-8418-665049CA220F}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
@@ -13640,6 +13621,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E509B35-A292-4896-84EE-9157D4436BDA}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -14435,6 +14417,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4D2FA8-D735-48AC-B928-6081B29FCD3B}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14880,6 +14863,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DF8194-EAB2-4AAC-9B35-F09487A4BBC8}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:Y103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -16933,6 +16917,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FEB92-3C8E-4A89-8F18-2AEFFF284423}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17167,7 +17152,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A846FF-BBF5-4A02-BAF4-3C4772884C84}">
-  <sheetPr>
+  <sheetPr codeName="Sheet9">
     <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:C2"/>

</xml_diff>

<commit_message>
Add fuel substitution in IND
</commit_message>
<xml_diff>
--- a/VT_IE_IND.xlsx
+++ b/VT_IE_IND.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gargiulo\Desktop\Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73803BCC-55BA-42AE-98F6-FDC67B333E7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1391D6FE-A4C6-47D8-8F5A-D5324CE40565}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -66,6 +66,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Maurizio Gargiulo</author>
+  </authors>
+  <commentList>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{AB4D4C44-2076-4F9F-86F2-6AED12743B8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Maurizio Gargiulo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bio Jet Kerosene. Should be reviewed?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{6CD33743-C0B5-4B36-95BB-0371E4D7E6F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Maurizio Gargiulo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The same as in transport</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -89,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="333">
   <si>
     <t>Development</t>
   </si>
@@ -1090,6 +1148,24 @@
   <si>
     <t>BIOMSW1,BIOMSW2</t>
   </si>
+  <si>
+    <t>BioDiesel (IND)</t>
+  </si>
+  <si>
+    <t>INDBDL</t>
+  </si>
+  <si>
+    <t>BIODST1G,BIODST2G</t>
+  </si>
+  <si>
+    <t>BioKerosene (IND)</t>
+  </si>
+  <si>
+    <t>INDBKE</t>
+  </si>
+  <si>
+    <t>BIOJKR</t>
+  </si>
 </sst>
 </file>
 
@@ -1103,7 +1179,7 @@
     <numFmt numFmtId="168" formatCode="\Te\x\t"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,6 +1302,44 @@
       <sz val="10"/>
       <name val="Myriad Pro"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3296,7 +3410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="333">
+  <cellXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4219,6 +4333,17 @@
     <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -12670,7 +12795,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="landscape" cellComments="asDisplayed" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" fitToHeight="0" orientation="landscape" cellComments="asDisplayed" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Myriad Pro,Regular"&amp;14Ireland's Energy Balance &amp;A</oddHeader>
     <oddFooter>&amp;L&amp;G&amp;RPage &amp;P of &amp;N</oddFooter>
@@ -12682,10 +12807,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1C8D34-EFD7-45C2-8418-665049CA220F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2:L43"/>
+  <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12817,27 +12942,27 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
     </row>
-    <row r="8" spans="2:12">
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="2:12" s="1" customFormat="1">
+      <c r="B8" s="333" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="26" t="str">
+      <c r="C8" s="333" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="F8" s="25" t="s">
+      <c r="D8" s="333" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8" s="333" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="333" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="G8" s="333"/>
+      <c r="H8" s="333"/>
+      <c r="I8" s="333"/>
+      <c r="J8" s="333"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="25" t="s">
@@ -12848,10 +12973,10 @@
         <v>IE,National</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>176</v>
@@ -12870,10 +12995,10 @@
         <v>IE,National</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F10" s="25" t="s">
         <v>176</v>
@@ -12892,10 +13017,10 @@
         <v>IE,National</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F11" s="25" t="s">
         <v>176</v>
@@ -12905,27 +13030,27 @@
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="2:12">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="2:12" s="1" customFormat="1">
+      <c r="B12" s="333" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="26" t="str">
+      <c r="C12" s="333" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="F12" s="25" t="s">
+      <c r="D12" s="333" t="s">
+        <v>328</v>
+      </c>
+      <c r="E12" s="333" t="s">
+        <v>327</v>
+      </c>
+      <c r="F12" s="333" t="s">
         <v>176</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="G12" s="333"/>
+      <c r="H12" s="333"/>
+      <c r="I12" s="333"/>
+      <c r="J12" s="333"/>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="25" t="s">
@@ -12936,18 +13061,16 @@
         <v>IE,National</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>215</v>
+        <v>273</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>176</v>
       </c>
       <c r="G13" s="25"/>
-      <c r="H13" s="25" t="s">
-        <v>244</v>
-      </c>
+      <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
     </row>
@@ -12960,10 +13083,10 @@
         <v>IE,National</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F14" s="25" t="s">
         <v>176</v>
@@ -12982,16 +13105,18 @@
         <v>IE,National</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>321</v>
+        <v>215</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>319</v>
+        <v>214</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>176</v>
       </c>
       <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="H15" s="25" t="s">
+        <v>244</v>
+      </c>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
     </row>
@@ -13004,10 +13129,10 @@
         <v>IE,National</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>322</v>
+        <v>217</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>320</v>
+        <v>218</v>
       </c>
       <c r="F16" s="25" t="s">
         <v>176</v>
@@ -13026,10 +13151,10 @@
         <v>IE,National</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>176</v>
@@ -13040,32 +13165,40 @@
       <c r="J17" s="25"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="B18" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="25" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="C19" s="26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A31)),SUBSTITUTE('EB2018'!A31,"&amp;","and"), 'EB2018'!A31) &amp; " demand"</f>
-        <v>Non-Energy Mining demand</v>
+        <v>323</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>216</v>
       </c>
       <c r="F19" s="25" t="s">
         <v>176</v>
@@ -13076,27 +13209,17 @@
       <c r="J19" s="25"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" s="26" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E20" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A32)),SUBSTITUTE('EB2018'!A32,"&amp;","and"), 'EB2018'!A32) &amp; " demand"</f>
-        <v>Food and beverages demand</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
+      <c r="B20" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="25" t="s">
@@ -13107,11 +13230,11 @@
         <v>IE,National</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E21" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A33)),SUBSTITUTE('EB2018'!A33,"&amp;","and"), 'EB2018'!A33) &amp; " demand"</f>
-        <v>Textiles and textile products demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A31)),SUBSTITUTE('EB2018'!A31,"&amp;","and"), 'EB2018'!A31) &amp; " demand"</f>
+        <v>Non-Energy Mining demand</v>
       </c>
       <c r="F21" s="25" t="s">
         <v>176</v>
@@ -13130,11 +13253,11 @@
         <v>IE,National</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E22" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A34)),SUBSTITUTE('EB2018'!A34,"&amp;","and"), 'EB2018'!A34) &amp; " demand"</f>
-        <v>Wood and wood products demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A32)),SUBSTITUTE('EB2018'!A32,"&amp;","and"), 'EB2018'!A32) &amp; " demand"</f>
+        <v>Food and beverages demand</v>
       </c>
       <c r="F22" s="25" t="s">
         <v>176</v>
@@ -13153,11 +13276,11 @@
         <v>IE,National</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E23" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A35)),SUBSTITUTE('EB2018'!A35,"&amp;","and"), 'EB2018'!A35) &amp; " demand"</f>
-        <v>Pulp, paper, publishing and printing demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A33)),SUBSTITUTE('EB2018'!A33,"&amp;","and"), 'EB2018'!A33) &amp; " demand"</f>
+        <v>Textiles and textile products demand</v>
       </c>
       <c r="F23" s="25" t="s">
         <v>176</v>
@@ -13176,11 +13299,11 @@
         <v>IE,National</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E24" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A36)),SUBSTITUTE('EB2018'!A36,"&amp;","and"), 'EB2018'!A36) &amp; " demand"</f>
-        <v>Chemicals and man-made fibres demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A34)),SUBSTITUTE('EB2018'!A34,"&amp;","and"), 'EB2018'!A34) &amp; " demand"</f>
+        <v>Wood and wood products demand</v>
       </c>
       <c r="F24" s="25" t="s">
         <v>176</v>
@@ -13199,11 +13322,11 @@
         <v>IE,National</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E25" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A37)),SUBSTITUTE('EB2018'!A37,"&amp;","and"), 'EB2018'!A37) &amp; " demand"</f>
-        <v>Rubber and plastic products demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A35)),SUBSTITUTE('EB2018'!A35,"&amp;","and"), 'EB2018'!A35) &amp; " demand"</f>
+        <v>Pulp, paper, publishing and printing demand</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>176</v>
@@ -13222,11 +13345,11 @@
         <v>IE,National</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E26" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A38)),SUBSTITUTE('EB2018'!A38,"&amp;","and"), 'EB2018'!A38) &amp; " demand"</f>
-        <v>Other non-metallic mineral products demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A36)),SUBSTITUTE('EB2018'!A36,"&amp;","and"), 'EB2018'!A36) &amp; " demand"</f>
+        <v>Chemicals and man-made fibres demand</v>
       </c>
       <c r="F26" s="25" t="s">
         <v>176</v>
@@ -13245,11 +13368,11 @@
         <v>IE,National</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E27" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A39)),SUBSTITUTE('EB2018'!A39,"&amp;","and"), 'EB2018'!A39) &amp; " demand"</f>
-        <v>Basic metals and fabricated metal products demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A37)),SUBSTITUTE('EB2018'!A37,"&amp;","and"), 'EB2018'!A37) &amp; " demand"</f>
+        <v>Rubber and plastic products demand</v>
       </c>
       <c r="F27" s="25" t="s">
         <v>176</v>
@@ -13268,11 +13391,11 @@
         <v>IE,National</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E28" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A40)),SUBSTITUTE('EB2018'!A40,"&amp;","and"), 'EB2018'!A40) &amp; " demand"</f>
-        <v>Machinery and equipment n.e.c. demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A38)),SUBSTITUTE('EB2018'!A38,"&amp;","and"), 'EB2018'!A38) &amp; " demand"</f>
+        <v>Other non-metallic mineral products demand</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>176</v>
@@ -13291,11 +13414,11 @@
         <v>IE,National</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E29" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A41)),SUBSTITUTE('EB2018'!A41,"&amp;","and"), 'EB2018'!A41) &amp; " demand"</f>
-        <v>Electrical and optical equipment demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A39)),SUBSTITUTE('EB2018'!A39,"&amp;","and"), 'EB2018'!A39) &amp; " demand"</f>
+        <v>Basic metals and fabricated metal products demand</v>
       </c>
       <c r="F29" s="25" t="s">
         <v>176</v>
@@ -13314,11 +13437,11 @@
         <v>IE,National</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E30" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A42)),SUBSTITUTE('EB2018'!A42,"&amp;","and"), 'EB2018'!A42) &amp; " demand"</f>
-        <v>Transport equipment manufacture demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A40)),SUBSTITUTE('EB2018'!A40,"&amp;","and"), 'EB2018'!A40) &amp; " demand"</f>
+        <v>Machinery and equipment n.e.c. demand</v>
       </c>
       <c r="F30" s="25" t="s">
         <v>176</v>
@@ -13337,11 +13460,11 @@
         <v>IE,National</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E31" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A43)),SUBSTITUTE('EB2018'!A43,"&amp;","and"), 'EB2018'!A43) &amp; " demand"</f>
-        <v>Other manufacturing demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A41)),SUBSTITUTE('EB2018'!A41,"&amp;","and"), 'EB2018'!A41) &amp; " demand"</f>
+        <v>Electrical and optical equipment demand</v>
       </c>
       <c r="F31" s="25" t="s">
         <v>176</v>
@@ -13360,11 +13483,11 @@
         <v>IE,National</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>318</v>
+        <v>233</v>
       </c>
       <c r="E32" s="28" t="str">
-        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A44)),SUBSTITUTE('EB2018'!A44,"&amp;","and"), 'EB2018'!A44) &amp; " demand"</f>
-        <v>Construction demand</v>
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A42)),SUBSTITUTE('EB2018'!A42,"&amp;","and"), 'EB2018'!A42) &amp; " demand"</f>
+        <v>Transport equipment manufacture demand</v>
       </c>
       <c r="F32" s="25" t="s">
         <v>176</v>
@@ -13375,34 +13498,45 @@
       <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
+      <c r="B33" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="E33" s="28" t="str">
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A43)),SUBSTITUTE('EB2018'!A43,"&amp;","and"), 'EB2018'!A43) &amp; " demand"</f>
+        <v>Other manufacturing demand</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="25" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="C34" s="26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>188</v>
+        <v>318</v>
+      </c>
+      <c r="E34" s="28" t="str">
+        <f>IF(ISNUMBER(SEARCH("&amp;",'EB2018'!A44)),SUBSTITUTE('EB2018'!A44,"&amp;","and"), 'EB2018'!A44) &amp; " demand"</f>
+        <v>Construction demand</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
@@ -13410,26 +13544,17 @@
       <c r="J34" s="25"/>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="C35" s="26" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
+      <c r="B35" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="25" t="s">
@@ -13440,10 +13565,10 @@
         <v>IE,National</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F36" s="25" t="s">
         <v>186</v>
@@ -13462,10 +13587,10 @@
         <v>IE,National</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F37" s="25" t="s">
         <v>186</v>
@@ -13484,10 +13609,10 @@
         <v>IE,National</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F38" s="25" t="s">
         <v>186</v>
@@ -13506,10 +13631,10 @@
         <v>IE,National</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>186</v>
@@ -13528,10 +13653,10 @@
         <v>IE,National</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F40" s="25" t="s">
         <v>186</v>
@@ -13550,10 +13675,10 @@
         <v>IE,National</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F41" s="25" t="s">
         <v>186</v>
@@ -13572,10 +13697,10 @@
         <v>IE,National</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F42" s="25" t="s">
         <v>186</v>
@@ -13594,10 +13719,10 @@
         <v>IE,National</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F43" s="25" t="s">
         <v>186</v>
@@ -13606,6 +13731,50 @@
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13615,10 +13784,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E509B35-A292-4896-84EE-9157D4436BDA}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:J32"/>
+  <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13695,11 +13864,11 @@
         <v>IE,National</v>
       </c>
       <c r="D5" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B5,MID(Commodities!D19,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B5,MID(Commodities!D21,2,3),"E0")</f>
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="E5" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E19," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E21," process")</f>
         <v>Non-Energy Mining demand process</v>
       </c>
       <c r="F5" s="29" t="s">
@@ -13721,11 +13890,11 @@
         <v>IE,National</v>
       </c>
       <c r="D6" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B6,MID(Commodities!D20,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B6,MID(Commodities!D22,2,3),"E0")</f>
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="E6" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E20," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E22," process")</f>
         <v>Food and beverages demand process</v>
       </c>
       <c r="F6" s="29" t="s">
@@ -13747,11 +13916,11 @@
         <v>IE,National</v>
       </c>
       <c r="D7" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B7,MID(Commodities!D21,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B7,MID(Commodities!D23,2,3),"E0")</f>
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="E7" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E21," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E23," process")</f>
         <v>Textiles and textile products demand process</v>
       </c>
       <c r="F7" s="29" t="s">
@@ -13773,11 +13942,11 @@
         <v>IE,National</v>
       </c>
       <c r="D8" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B8,MID(Commodities!D22,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B8,MID(Commodities!D24,2,3),"E0")</f>
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="E8" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E22," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E24," process")</f>
         <v>Wood and wood products demand process</v>
       </c>
       <c r="F8" s="29" t="s">
@@ -13799,11 +13968,11 @@
         <v>IE,National</v>
       </c>
       <c r="D9" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B9,MID(Commodities!D23,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B9,MID(Commodities!D25,2,3),"E0")</f>
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="E9" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E23," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E25," process")</f>
         <v>Pulp, paper, publishing and printing demand process</v>
       </c>
       <c r="F9" s="29" t="s">
@@ -13825,11 +13994,11 @@
         <v>IE,National</v>
       </c>
       <c r="D10" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B10,MID(Commodities!D24,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B10,MID(Commodities!D26,2,3),"E0")</f>
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="E10" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E24," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E26," process")</f>
         <v>Chemicals and man-made fibres demand process</v>
       </c>
       <c r="F10" s="29" t="s">
@@ -13851,11 +14020,11 @@
         <v>IE,National</v>
       </c>
       <c r="D11" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B11,MID(Commodities!D25,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B11,MID(Commodities!D27,2,3),"E0")</f>
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="E11" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E25," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E27," process")</f>
         <v>Rubber and plastic products demand process</v>
       </c>
       <c r="F11" s="29" t="s">
@@ -13877,11 +14046,11 @@
         <v>IE,National</v>
       </c>
       <c r="D12" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B12,MID(Commodities!D26,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B12,MID(Commodities!D28,2,3),"E0")</f>
         <v>I-DMD-ONM-E0</v>
       </c>
       <c r="E12" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E26," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E28," process")</f>
         <v>Other non-metallic mineral products demand process</v>
       </c>
       <c r="F12" s="29" t="s">
@@ -13903,11 +14072,11 @@
         <v>IE,National</v>
       </c>
       <c r="D13" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B13,MID(Commodities!D27,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B13,MID(Commodities!D29,2,3),"E0")</f>
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="E13" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E27," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E29," process")</f>
         <v>Basic metals and fabricated metal products demand process</v>
       </c>
       <c r="F13" s="29" t="s">
@@ -13929,11 +14098,11 @@
         <v>IE,National</v>
       </c>
       <c r="D14" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B14,MID(Commodities!D28,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B14,MID(Commodities!D30,2,3),"E0")</f>
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="E14" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E28," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E30," process")</f>
         <v>Machinery and equipment n.e.c. demand process</v>
       </c>
       <c r="F14" s="29" t="s">
@@ -13955,11 +14124,11 @@
         <v>IE,National</v>
       </c>
       <c r="D15" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B15,MID(Commodities!D29,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B15,MID(Commodities!D31,2,3),"E0")</f>
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="E15" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E29," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E31," process")</f>
         <v>Electrical and optical equipment demand process</v>
       </c>
       <c r="F15" s="29" t="s">
@@ -13981,11 +14150,11 @@
         <v>IE,National</v>
       </c>
       <c r="D16" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B16,MID(Commodities!D30,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B16,MID(Commodities!D32,2,3),"E0")</f>
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="E16" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E30," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E32," process")</f>
         <v>Transport equipment manufacture demand process</v>
       </c>
       <c r="F16" s="32" t="s">
@@ -14007,11 +14176,11 @@
         <v>IE,National</v>
       </c>
       <c r="D17" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B17,MID(Commodities!D31,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B17,MID(Commodities!D33,2,3),"E0")</f>
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="E17" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E31," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E33," process")</f>
         <v>Other manufacturing demand process</v>
       </c>
       <c r="F17" s="29" t="s">
@@ -14033,11 +14202,11 @@
         <v>IE,National</v>
       </c>
       <c r="D18" s="26" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B18,MID(Commodities!D32,2,3),"E0")</f>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"I",B18,MID(Commodities!D34,2,3),"E0")</f>
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="E18" s="26" t="str">
-        <f>_xlfn.CONCAT(Commodities!E32," process")</f>
+        <f>_xlfn.CONCAT(Commodities!E34," process")</f>
         <v>Construction demand process</v>
       </c>
       <c r="F18" s="29" t="s">
@@ -14141,26 +14310,26 @@
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="2:10" s="1" customFormat="1">
+      <c r="B23" s="333" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="26" t="str">
+      <c r="C23" s="333" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D23" s="26" t="str">
+      <c r="D23" s="333" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D8)</f>
-        <v>FT-INDHFO</v>
-      </c>
-      <c r="E23" s="26" t="str">
+        <v>FT-INDBKE</v>
+      </c>
+      <c r="E23" s="333" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E8)</f>
-        <v>Fuel Tech - Heavy Fuel Oil (IND)</v>
-      </c>
-      <c r="F23" s="35" t="s">
+        <v>Fuel Tech - BioKerosene (IND)</v>
+      </c>
+      <c r="F23" s="334" t="s">
         <v>176</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="333" t="s">
         <v>247</v>
       </c>
       <c r="H23" s="32"/>
@@ -14177,11 +14346,11 @@
       </c>
       <c r="D24" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D9)</f>
-        <v>FT-INDLPG</v>
+        <v>FT-INDHFO</v>
       </c>
       <c r="E24" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E9)</f>
-        <v>Fuel Tech - Liquified Petroleum Gas (IND)</v>
+        <v>Fuel Tech - Heavy Fuel Oil (IND)</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>176</v>
@@ -14203,11 +14372,11 @@
       </c>
       <c r="D25" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D10)</f>
-        <v>FT-INDDST</v>
+        <v>FT-INDLPG</v>
       </c>
       <c r="E25" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E10)</f>
-        <v>Fuel Tech - Diesel (IND)</v>
+        <v>Fuel Tech - Liquified Petroleum Gas (IND)</v>
       </c>
       <c r="F25" s="35" t="s">
         <v>176</v>
@@ -14229,11 +14398,11 @@
       </c>
       <c r="D26" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D11)</f>
-        <v>FT-INDCOK</v>
+        <v>FT-INDDST</v>
       </c>
       <c r="E26" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E11)</f>
-        <v>Fuel Tech - Petroleum Coke (IND)</v>
+        <v>Fuel Tech - Diesel (IND)</v>
       </c>
       <c r="F26" s="35" t="s">
         <v>176</v>
@@ -14245,31 +14414,31 @@
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
     </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="26" t="s">
+    <row r="27" spans="2:10" s="1" customFormat="1">
+      <c r="B27" s="333" t="s">
         <v>245</v>
       </c>
-      <c r="C27" s="26" t="str">
+      <c r="C27" s="333" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D27" s="26" t="str">
+      <c r="D27" s="333" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D12)</f>
-        <v>FT-INDGAS</v>
-      </c>
-      <c r="E27" s="26" t="str">
+        <v>FT-INDBDL</v>
+      </c>
+      <c r="E27" s="333" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E12)</f>
-        <v>Fuel Tech - Natural Gas (IND)</v>
-      </c>
-      <c r="F27" s="35" t="s">
+        <v>Fuel Tech - BioDiesel (IND)</v>
+      </c>
+      <c r="F27" s="334" t="s">
         <v>176</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="333" t="s">
         <v>247</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="H27" s="335"/>
+      <c r="I27" s="336"/>
+      <c r="J27" s="336"/>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="26" t="s">
@@ -14281,11 +14450,11 @@
       </c>
       <c r="D28" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D13)</f>
-        <v>FT-INDELC</v>
+        <v>FT-INDCOK</v>
       </c>
       <c r="E28" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E13)</f>
-        <v>Fuel Tech - Electricity (IND)</v>
+        <v>Fuel Tech - Petroleum Coke (IND)</v>
       </c>
       <c r="F28" s="35" t="s">
         <v>176</v>
@@ -14293,9 +14462,7 @@
       <c r="G28" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H28" s="36" t="s">
-        <v>244</v>
-      </c>
+      <c r="H28" s="32"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
     </row>
@@ -14309,11 +14476,11 @@
       </c>
       <c r="D29" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D14)</f>
-        <v>FT-INDBGS</v>
+        <v>FT-INDGAS</v>
       </c>
       <c r="E29" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E14)</f>
-        <v>Fuel Tech - Biogas (IND)</v>
+        <v>Fuel Tech - Natural Gas (IND)</v>
       </c>
       <c r="F29" s="35" t="s">
         <v>176</v>
@@ -14321,7 +14488,7 @@
       <c r="G29" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H29" s="36"/>
+      <c r="H29" s="32"/>
       <c r="I29" s="36"/>
       <c r="J29" s="36"/>
     </row>
@@ -14335,11 +14502,11 @@
       </c>
       <c r="D30" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D15)</f>
-        <v>FT-INDBIO</v>
+        <v>FT-INDELC</v>
       </c>
       <c r="E30" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E15)</f>
-        <v>Fuel Tech - Biomass (IND)</v>
+        <v>Fuel Tech - Electricity (IND)</v>
       </c>
       <c r="F30" s="35" t="s">
         <v>176</v>
@@ -14347,7 +14514,9 @@
       <c r="G30" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H30" s="36"/>
+      <c r="H30" s="36" t="s">
+        <v>244</v>
+      </c>
       <c r="I30" s="36"/>
       <c r="J30" s="36"/>
     </row>
@@ -14361,11 +14530,11 @@
       </c>
       <c r="D31" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D16)</f>
-        <v>FT-INDRWS</v>
+        <v>FT-INDBGS</v>
       </c>
       <c r="E31" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E16)</f>
-        <v>Fuel Tech - Renewable waste (IND)</v>
+        <v>Fuel Tech - Biogas (IND)</v>
       </c>
       <c r="F31" s="35" t="s">
         <v>176</v>
@@ -14387,11 +14556,11 @@
       </c>
       <c r="D32" s="26" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D17)</f>
-        <v>FT-INDNWS</v>
+        <v>FT-INDBIO</v>
       </c>
       <c r="E32" s="26" t="str">
         <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E17)</f>
-        <v>Fuel Tech - Non-renewable waste (IND)</v>
+        <v>Fuel Tech - Biomass (IND)</v>
       </c>
       <c r="F32" s="35" t="s">
         <v>176</v>
@@ -14402,6 +14571,58 @@
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
       <c r="J32" s="36"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C33" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D33" s="26" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D18)</f>
+        <v>FT-INDRWS</v>
+      </c>
+      <c r="E33" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E18)</f>
+        <v>Fuel Tech - Renewable waste (IND)</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C34" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D34" s="26" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D19)</f>
+        <v>FT-INDNWS</v>
+      </c>
+      <c r="E34" s="26" t="str">
+        <f>_xlfn.TEXTJOIN(" - ",TRUE,"Fuel Tech",Commodities!E19)</f>
+        <v>Fuel Tech - Non-renewable waste (IND)</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14409,12 +14630,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4D2FA8-D735-48AC-B928-6081B29FCD3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4D2FA8-D735-48AC-B928-6081B29FCD3B}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14578,30 +14799,30 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
-      <c r="B9" t="str">
+    <row r="9" spans="2:8" s="1" customFormat="1">
+      <c r="B9" s="337" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="C9" s="40" t="str">
+      <c r="C9" s="338" t="str">
         <f>Processes!D23</f>
-        <v>FT-INDHFO</v>
-      </c>
-      <c r="D9" s="40" t="str">
+        <v>FT-INDBKE</v>
+      </c>
+      <c r="D9" s="338" t="str">
         <f>Processes!E23</f>
-        <v>Fuel Tech - Heavy Fuel Oil (IND)</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="40" t="str">
+        <v>Fuel Tech - BioKerosene (IND)</v>
+      </c>
+      <c r="E9" s="339" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" s="338" t="str">
         <f>Commodities!D8</f>
-        <v>INDHFO</v>
-      </c>
-      <c r="G9" s="45">
+        <v>INDBKE</v>
+      </c>
+      <c r="G9" s="339">
         <v>1</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="339">
         <v>50</v>
       </c>
     </row>
@@ -14612,18 +14833,18 @@
       </c>
       <c r="C10" s="40" t="str">
         <f>Processes!D24</f>
-        <v>FT-INDLPG</v>
+        <v>FT-INDHFO</v>
       </c>
       <c r="D10" s="40" t="str">
         <f>Processes!E24</f>
-        <v>Fuel Tech - Liquified Petroleum Gas (IND)</v>
+        <v>Fuel Tech - Heavy Fuel Oil (IND)</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F10" s="40" t="str">
         <f>Commodities!D9</f>
-        <v>INDLPG</v>
+        <v>INDHFO</v>
       </c>
       <c r="G10" s="45">
         <v>1</v>
@@ -14639,18 +14860,18 @@
       </c>
       <c r="C11" s="40" t="str">
         <f>Processes!D25</f>
-        <v>FT-INDDST</v>
+        <v>FT-INDLPG</v>
       </c>
       <c r="D11" s="40" t="str">
         <f>Processes!E25</f>
-        <v>Fuel Tech - Diesel (IND)</v>
+        <v>Fuel Tech - Liquified Petroleum Gas (IND)</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F11" s="40" t="str">
         <f>Commodities!D10</f>
-        <v>INDDST</v>
+        <v>INDLPG</v>
       </c>
       <c r="G11" s="45">
         <v>1</v>
@@ -14666,18 +14887,18 @@
       </c>
       <c r="C12" s="40" t="str">
         <f>Processes!D26</f>
-        <v>FT-INDCOK</v>
+        <v>FT-INDDST</v>
       </c>
       <c r="D12" s="40" t="str">
         <f>Processes!E26</f>
-        <v>Fuel Tech - Petroleum Coke (IND)</v>
+        <v>Fuel Tech - Diesel (IND)</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F12" s="40" t="str">
         <f>Commodities!D11</f>
-        <v>INDCOK</v>
+        <v>INDDST</v>
       </c>
       <c r="G12" s="45">
         <v>1</v>
@@ -14686,30 +14907,30 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
-      <c r="B13" t="str">
+    <row r="13" spans="2:8" s="1" customFormat="1">
+      <c r="B13" s="337" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="C13" s="40" t="str">
+      <c r="C13" s="338" t="str">
         <f>Processes!D27</f>
-        <v>FT-INDGAS</v>
-      </c>
-      <c r="D13" s="40" t="str">
+        <v>FT-INDBDL</v>
+      </c>
+      <c r="D13" s="338" t="str">
         <f>Processes!E27</f>
-        <v>Fuel Tech - Natural Gas (IND)</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="F13" s="40" t="str">
+        <v>Fuel Tech - BioDiesel (IND)</v>
+      </c>
+      <c r="E13" s="339" t="s">
+        <v>329</v>
+      </c>
+      <c r="F13" s="338" t="str">
         <f>Commodities!D12</f>
-        <v>INDGAS</v>
-      </c>
-      <c r="G13" s="45">
+        <v>INDBDL</v>
+      </c>
+      <c r="G13" s="339">
         <v>1</v>
       </c>
-      <c r="H13" s="45">
+      <c r="H13" s="339">
         <v>50</v>
       </c>
     </row>
@@ -14720,18 +14941,18 @@
       </c>
       <c r="C14" s="40" t="str">
         <f>Processes!D28</f>
-        <v>FT-INDELC</v>
+        <v>FT-INDCOK</v>
       </c>
       <c r="D14" s="40" t="str">
         <f>Processes!E28</f>
-        <v>Fuel Tech - Electricity (IND)</v>
+        <v>Fuel Tech - Petroleum Coke (IND)</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>266</v>
+        <v>182</v>
       </c>
       <c r="F14" s="40" t="str">
         <f>Commodities!D13</f>
-        <v>INDELC</v>
+        <v>INDCOK</v>
       </c>
       <c r="G14" s="45">
         <v>1</v>
@@ -14747,18 +14968,18 @@
       </c>
       <c r="C15" s="40" t="str">
         <f>Processes!D29</f>
-        <v>FT-INDBGS</v>
+        <v>FT-INDGAS</v>
       </c>
       <c r="D15" s="40" t="str">
         <f>Processes!E29</f>
-        <v>Fuel Tech - Biogas (IND)</v>
+        <v>Fuel Tech - Natural Gas (IND)</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>263</v>
+        <v>183</v>
       </c>
       <c r="F15" s="40" t="str">
         <f>Commodities!D14</f>
-        <v>INDBGS</v>
+        <v>INDGAS</v>
       </c>
       <c r="G15" s="45">
         <v>1</v>
@@ -14774,18 +14995,18 @@
       </c>
       <c r="C16" s="40" t="str">
         <f>Processes!D30</f>
-        <v>FT-INDBIO</v>
+        <v>FT-INDELC</v>
       </c>
       <c r="D16" s="40" t="str">
         <f>Processes!E30</f>
-        <v>Fuel Tech - Biomass (IND)</v>
+        <v>Fuel Tech - Electricity (IND)</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>324</v>
+        <v>266</v>
       </c>
       <c r="F16" s="40" t="str">
         <f>Commodities!D15</f>
-        <v>INDBIO</v>
+        <v>INDELC</v>
       </c>
       <c r="G16" s="45">
         <v>1</v>
@@ -14801,18 +15022,18 @@
       </c>
       <c r="C17" s="40" t="str">
         <f>Processes!D31</f>
-        <v>FT-INDRWS</v>
+        <v>FT-INDBGS</v>
       </c>
       <c r="D17" s="40" t="str">
         <f>Processes!E31</f>
-        <v>Fuel Tech - Renewable waste (IND)</v>
+        <v>Fuel Tech - Biogas (IND)</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>325</v>
+        <v>263</v>
       </c>
       <c r="F17" s="40" t="str">
         <f>Commodities!D16</f>
-        <v>INDRWS</v>
+        <v>INDBGS</v>
       </c>
       <c r="G17" s="45">
         <v>1</v>
@@ -14828,18 +15049,18 @@
       </c>
       <c r="C18" s="40" t="str">
         <f>Processes!D32</f>
-        <v>FT-INDNWS</v>
+        <v>FT-INDBIO</v>
       </c>
       <c r="D18" s="40" t="str">
         <f>Processes!E32</f>
-        <v>Fuel Tech - Non-renewable waste (IND)</v>
+        <v>Fuel Tech - Biomass (IND)</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F18" s="40" t="str">
         <f>Commodities!D17</f>
-        <v>INDNWS</v>
+        <v>INDBIO</v>
       </c>
       <c r="G18" s="45">
         <v>1</v>
@@ -14847,10 +15068,69 @@
       <c r="H18" s="45">
         <v>50</v>
       </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C19" s="40" t="str">
+        <f>Processes!D33</f>
+        <v>FT-INDRWS</v>
+      </c>
+      <c r="D19" s="40" t="str">
+        <f>Processes!E33</f>
+        <v>Fuel Tech - Renewable waste (IND)</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="F19" s="40" t="str">
+        <f>Commodities!D18</f>
+        <v>INDRWS</v>
+      </c>
+      <c r="G19" s="45">
+        <v>1</v>
+      </c>
+      <c r="H19" s="45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="C20" s="40" t="str">
+        <f>Processes!D34</f>
+        <v>FT-INDNWS</v>
+      </c>
+      <c r="D20" s="40" t="str">
+        <f>Processes!E34</f>
+        <v>Fuel Tech - Non-renewable waste (IND)</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="F20" s="40" t="str">
+        <f>Commodities!D19</f>
+        <v>INDNWS</v>
+      </c>
+      <c r="G20" s="45">
+        <v>1</v>
+      </c>
+      <c r="H20" s="45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14859,8 +15139,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:Y103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14976,7 +15256,7 @@
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="40" t="str">
-        <f>Commodities!D19</f>
+        <f>Commodities!D21</f>
         <v>INEM</v>
       </c>
       <c r="G6" s="45">
@@ -15035,7 +15315,7 @@
       <c r="C8" s="40"/>
       <c r="D8" s="40"/>
       <c r="E8" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F8" s="40"/>
@@ -15066,7 +15346,7 @@
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
       <c r="E9" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F9" s="40"/>
@@ -15097,7 +15377,7 @@
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
       <c r="E10" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F10" s="40"/>
@@ -15129,7 +15409,7 @@
       <c r="C11" s="42"/>
       <c r="D11" s="42"/>
       <c r="E11" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F11" s="42"/>
@@ -15174,7 +15454,7 @@
         <v>INDCOA</v>
       </c>
       <c r="F12" s="40" t="str">
-        <f>Commodities!D20</f>
+        <f>Commodities!D22</f>
         <v>IFAB</v>
       </c>
       <c r="G12" s="45">
@@ -15232,7 +15512,7 @@
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="41" t="str">
-        <f>Commodities!$D$8</f>
+        <f>Commodities!$D$9</f>
         <v>INDHFO</v>
       </c>
       <c r="F15" s="40"/>
@@ -15250,7 +15530,7 @@
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F16" s="40"/>
@@ -15268,7 +15548,7 @@
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F17" s="40"/>
@@ -15286,7 +15566,7 @@
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
       <c r="E18" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F18" s="40"/>
@@ -15304,7 +15584,7 @@
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="41" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F19" s="40"/>
@@ -15322,7 +15602,7 @@
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="41" t="str">
-        <f>Commodities!$D$14</f>
+        <f>Commodities!$D$16</f>
         <v>INDBGS</v>
       </c>
       <c r="F20" s="40"/>
@@ -15341,7 +15621,7 @@
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
       <c r="E21" s="43" t="str">
-        <f>Commodities!$D$15</f>
+        <f>Commodities!$D$17</f>
         <v>INDBIO</v>
       </c>
       <c r="F21" s="42"/>
@@ -15370,7 +15650,7 @@
       </c>
       <c r="E22" s="41"/>
       <c r="F22" s="40" t="str">
-        <f>Commodities!D21</f>
+        <f>Commodities!D23</f>
         <v>ITAP</v>
       </c>
       <c r="G22" s="45">
@@ -15403,7 +15683,7 @@
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F24" s="40"/>
@@ -15421,7 +15701,7 @@
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
       <c r="E25" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F25" s="40"/>
@@ -15439,7 +15719,7 @@
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
       <c r="E26" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F26" s="40"/>
@@ -15458,7 +15738,7 @@
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
       <c r="E27" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F27" s="42"/>
@@ -15487,7 +15767,7 @@
       </c>
       <c r="E28" s="41"/>
       <c r="F28" s="40" t="str">
-        <f>Commodities!D22</f>
+        <f>Commodities!D24</f>
         <v>IWAP</v>
       </c>
       <c r="G28" s="45">
@@ -15520,7 +15800,7 @@
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
       <c r="E30" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F30" s="40"/>
@@ -15538,7 +15818,7 @@
       <c r="C31" s="40"/>
       <c r="D31" s="40"/>
       <c r="E31" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F31" s="40"/>
@@ -15556,7 +15836,7 @@
       <c r="C32" s="40"/>
       <c r="D32" s="40"/>
       <c r="E32" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F32" s="40"/>
@@ -15574,7 +15854,7 @@
       <c r="C33" s="40"/>
       <c r="D33" s="40"/>
       <c r="E33" s="41" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F33" s="40"/>
@@ -15593,7 +15873,7 @@
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
       <c r="E34" s="43" t="str">
-        <f>Commodities!$D$15</f>
+        <f>Commodities!$D$17</f>
         <v>INDBIO</v>
       </c>
       <c r="F34" s="42"/>
@@ -15622,7 +15902,7 @@
       </c>
       <c r="E35" s="41"/>
       <c r="F35" s="40" t="str">
-        <f>Commodities!D23</f>
+        <f>Commodities!D25</f>
         <v>IPX4</v>
       </c>
       <c r="G35" s="45">
@@ -15655,7 +15935,7 @@
       <c r="C37" s="40"/>
       <c r="D37" s="40"/>
       <c r="E37" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F37" s="40"/>
@@ -15673,7 +15953,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="40"/>
       <c r="E38" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F38" s="40"/>
@@ -15691,7 +15971,7 @@
       <c r="C39" s="40"/>
       <c r="D39" s="40"/>
       <c r="E39" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F39" s="40"/>
@@ -15710,7 +15990,7 @@
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
       <c r="E40" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F40" s="42"/>
@@ -15739,7 +16019,7 @@
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="40" t="str">
-        <f>Commodities!D24</f>
+        <f>Commodities!D26</f>
         <v>ICAF</v>
       </c>
       <c r="G41" s="45">
@@ -15772,7 +16052,7 @@
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="41" t="str">
-        <f>Commodities!$D$8</f>
+        <f>Commodities!$D$9</f>
         <v>INDHFO</v>
       </c>
       <c r="F43" s="40"/>
@@ -15790,7 +16070,7 @@
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
       <c r="E44" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F44" s="40"/>
@@ -15808,7 +16088,7 @@
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
       <c r="E45" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F45" s="40"/>
@@ -15826,7 +16106,7 @@
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
       <c r="E46" s="41" t="str">
-        <f>Commodities!$D$11</f>
+        <f>Commodities!$D$13</f>
         <v>INDCOK</v>
       </c>
       <c r="F46" s="40"/>
@@ -15844,7 +16124,7 @@
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
       <c r="E47" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F47" s="40"/>
@@ -15863,7 +16143,7 @@
       <c r="C48" s="42"/>
       <c r="D48" s="42"/>
       <c r="E48" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F48" s="42"/>
@@ -15892,7 +16172,7 @@
       </c>
       <c r="E49" s="41"/>
       <c r="F49" s="40" t="str">
-        <f>Commodities!D25</f>
+        <f>Commodities!D27</f>
         <v>IRAP</v>
       </c>
       <c r="G49" s="45">
@@ -15925,7 +16205,7 @@
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
       <c r="E51" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F51" s="40"/>
@@ -15943,7 +16223,7 @@
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
       <c r="E52" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F52" s="40"/>
@@ -15961,7 +16241,7 @@
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
       <c r="E53" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F53" s="40"/>
@@ -15980,7 +16260,7 @@
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
       <c r="E54" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F54" s="42"/>
@@ -16012,7 +16292,7 @@
         <v>INDCOA</v>
       </c>
       <c r="F55" s="40" t="str">
-        <f>Commodities!D26</f>
+        <f>Commodities!D28</f>
         <v>IONM</v>
       </c>
       <c r="G55" s="45">
@@ -16051,7 +16331,7 @@
       <c r="C57" s="40"/>
       <c r="D57" s="40"/>
       <c r="E57" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F57" s="40"/>
@@ -16069,7 +16349,7 @@
       <c r="C58" s="40"/>
       <c r="D58" s="40"/>
       <c r="E58" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F58" s="40"/>
@@ -16087,7 +16367,7 @@
       <c r="C59" s="40"/>
       <c r="D59" s="40"/>
       <c r="E59" s="41" t="str">
-        <f>Commodities!$D$11</f>
+        <f>Commodities!$D$13</f>
         <v>INDCOK</v>
       </c>
       <c r="F59" s="40"/>
@@ -16105,7 +16385,7 @@
       <c r="C60" s="40"/>
       <c r="D60" s="40"/>
       <c r="E60" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F60" s="40"/>
@@ -16123,7 +16403,7 @@
       <c r="C61" s="40"/>
       <c r="D61" s="40"/>
       <c r="E61" s="41" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F61" s="40"/>
@@ -16141,7 +16421,7 @@
       <c r="C62" s="40"/>
       <c r="D62" s="40"/>
       <c r="E62" s="41" t="str">
-        <f>Commodities!$D$15</f>
+        <f>Commodities!$D$17</f>
         <v>INDBIO</v>
       </c>
       <c r="F62" s="40"/>
@@ -16159,7 +16439,7 @@
       <c r="C63" s="40"/>
       <c r="D63" s="40"/>
       <c r="E63" s="41" t="str">
-        <f>Commodities!$D$16</f>
+        <f>Commodities!$D$18</f>
         <v>INDRWS</v>
       </c>
       <c r="F63" s="40"/>
@@ -16178,7 +16458,7 @@
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="43" t="str">
-        <f>Commodities!$D$17</f>
+        <f>Commodities!$D$19</f>
         <v>INDNWS</v>
       </c>
       <c r="F64" s="42"/>
@@ -16207,7 +16487,7 @@
       </c>
       <c r="E65" s="41"/>
       <c r="F65" s="40" t="str">
-        <f>Commodities!D27</f>
+        <f>Commodities!D29</f>
         <v>IMAP</v>
       </c>
       <c r="G65" s="45">
@@ -16258,7 +16538,7 @@
       <c r="C68" s="40"/>
       <c r="D68" s="40"/>
       <c r="E68" s="41" t="str">
-        <f>Commodities!$D$8</f>
+        <f>Commodities!$D$9</f>
         <v>INDHFO</v>
       </c>
       <c r="F68" s="40"/>
@@ -16276,7 +16556,7 @@
       <c r="C69" s="40"/>
       <c r="D69" s="40"/>
       <c r="E69" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F69" s="40"/>
@@ -16294,7 +16574,7 @@
       <c r="C70" s="40"/>
       <c r="D70" s="40"/>
       <c r="E70" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F70" s="40"/>
@@ -16312,7 +16592,7 @@
       <c r="C71" s="40"/>
       <c r="D71" s="40"/>
       <c r="E71" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F71" s="40"/>
@@ -16331,7 +16611,7 @@
       <c r="C72" s="42"/>
       <c r="D72" s="42"/>
       <c r="E72" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F72" s="42"/>
@@ -16360,7 +16640,7 @@
       </c>
       <c r="E73" s="41"/>
       <c r="F73" s="40" t="str">
-        <f>Commodities!D28</f>
+        <f>Commodities!D30</f>
         <v>IMAE</v>
       </c>
       <c r="G73" s="45">
@@ -16393,7 +16673,7 @@
       <c r="C75" s="40"/>
       <c r="D75" s="40"/>
       <c r="E75" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F75" s="40"/>
@@ -16411,7 +16691,7 @@
       <c r="C76" s="40"/>
       <c r="D76" s="40"/>
       <c r="E76" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F76" s="40"/>
@@ -16429,7 +16709,7 @@
       <c r="C77" s="40"/>
       <c r="D77" s="40"/>
       <c r="E77" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F77" s="40"/>
@@ -16448,7 +16728,7 @@
       <c r="C78" s="42"/>
       <c r="D78" s="42"/>
       <c r="E78" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F78" s="42"/>
@@ -16477,7 +16757,7 @@
       </c>
       <c r="E79" s="41"/>
       <c r="F79" s="40" t="str">
-        <f>Commodities!D29</f>
+        <f>Commodities!D31</f>
         <v>IEOE</v>
       </c>
       <c r="G79" s="45">
@@ -16510,7 +16790,7 @@
       <c r="C81" s="40"/>
       <c r="D81" s="40"/>
       <c r="E81" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F81" s="40"/>
@@ -16528,7 +16808,7 @@
       <c r="C82" s="40"/>
       <c r="D82" s="40"/>
       <c r="E82" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F82" s="40"/>
@@ -16546,7 +16826,7 @@
       <c r="C83" s="40"/>
       <c r="D83" s="40"/>
       <c r="E83" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F83" s="40"/>
@@ -16565,7 +16845,7 @@
       <c r="C84" s="42"/>
       <c r="D84" s="42"/>
       <c r="E84" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F84" s="42"/>
@@ -16594,7 +16874,7 @@
       </c>
       <c r="E85" s="41"/>
       <c r="F85" s="40" t="str">
-        <f>Commodities!D30</f>
+        <f>Commodities!D32</f>
         <v>ITEM</v>
       </c>
       <c r="G85" s="45">
@@ -16627,7 +16907,7 @@
       <c r="C87" s="40"/>
       <c r="D87" s="40"/>
       <c r="E87" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="F87" s="40"/>
@@ -16645,7 +16925,7 @@
       <c r="C88" s="40"/>
       <c r="D88" s="40"/>
       <c r="E88" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="F88" s="40"/>
@@ -16663,7 +16943,7 @@
       <c r="C89" s="40"/>
       <c r="D89" s="40"/>
       <c r="E89" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="F89" s="40"/>
@@ -16682,7 +16962,7 @@
       <c r="C90" s="42"/>
       <c r="D90" s="42"/>
       <c r="E90" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F90" s="42"/>
@@ -16711,7 +16991,7 @@
       </c>
       <c r="E91" s="41"/>
       <c r="F91" s="40" t="str">
-        <f>Commodities!D31</f>
+        <f>Commodities!D33</f>
         <v>IOMA</v>
       </c>
       <c r="G91" s="45">
@@ -16737,7 +17017,7 @@
     </row>
     <row r="93" spans="2:10">
       <c r="E93" s="41" t="str">
-        <f>Commodities!$D$8</f>
+        <f>Commodities!$D$9</f>
         <v>INDHFO</v>
       </c>
       <c r="I93">
@@ -16750,7 +17030,7 @@
     </row>
     <row r="94" spans="2:10">
       <c r="E94" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="I94">
@@ -16763,7 +17043,7 @@
     </row>
     <row r="95" spans="2:10">
       <c r="E95" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="I95">
@@ -16776,7 +17056,7 @@
     </row>
     <row r="96" spans="2:10">
       <c r="E96" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="I96">
@@ -16792,7 +17072,7 @@
       <c r="C97" s="48"/>
       <c r="D97" s="48"/>
       <c r="E97" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F97" s="48"/>
@@ -16821,7 +17101,7 @@
       </c>
       <c r="E98" s="41"/>
       <c r="F98" s="40" t="str">
-        <f>Commodities!D32</f>
+        <f>Commodities!D34</f>
         <v>ICON</v>
       </c>
       <c r="G98" s="45">
@@ -16847,7 +17127,7 @@
     </row>
     <row r="100" spans="2:10">
       <c r="E100" s="41" t="str">
-        <f>Commodities!$D$9</f>
+        <f>Commodities!$D$10</f>
         <v>INDLPG</v>
       </c>
       <c r="I100">
@@ -16860,7 +17140,7 @@
     </row>
     <row r="101" spans="2:10">
       <c r="E101" s="41" t="str">
-        <f>Commodities!$D$10</f>
+        <f>Commodities!$D$11</f>
         <v>INDDST</v>
       </c>
       <c r="I101">
@@ -16873,7 +17153,7 @@
     </row>
     <row r="102" spans="2:10">
       <c r="E102" s="41" t="str">
-        <f>Commodities!$D$12</f>
+        <f>Commodities!$D$14</f>
         <v>INDGAS</v>
       </c>
       <c r="I102">
@@ -16889,7 +17169,7 @@
       <c r="C103" s="48"/>
       <c r="D103" s="48"/>
       <c r="E103" s="43" t="str">
-        <f>Commodities!$D$13</f>
+        <f>Commodities!$D$15</f>
         <v>INDELC</v>
       </c>
       <c r="F103" s="48"/>
@@ -16944,7 +17224,7 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="str">
-        <f>Commodities!D19</f>
+        <f>Commodities!D21</f>
         <v>INEM</v>
       </c>
       <c r="C4" s="37">
@@ -16958,7 +17238,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="str">
-        <f>Commodities!D20</f>
+        <f>Commodities!D22</f>
         <v>IFAB</v>
       </c>
       <c r="C5" s="37">
@@ -16972,7 +17252,7 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="str">
-        <f>Commodities!D21</f>
+        <f>Commodities!D23</f>
         <v>ITAP</v>
       </c>
       <c r="C6" s="37">
@@ -16986,7 +17266,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="str">
-        <f>Commodities!D22</f>
+        <f>Commodities!D24</f>
         <v>IWAP</v>
       </c>
       <c r="C7" s="37">
@@ -17000,7 +17280,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="str">
-        <f>Commodities!D23</f>
+        <f>Commodities!D25</f>
         <v>IPX4</v>
       </c>
       <c r="C8" s="37">
@@ -17014,7 +17294,7 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="str">
-        <f>Commodities!D24</f>
+        <f>Commodities!D26</f>
         <v>ICAF</v>
       </c>
       <c r="C9" s="37">
@@ -17028,7 +17308,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="str">
-        <f>Commodities!D25</f>
+        <f>Commodities!D27</f>
         <v>IRAP</v>
       </c>
       <c r="C10" s="37">
@@ -17042,7 +17322,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="str">
-        <f>Commodities!D26</f>
+        <f>Commodities!D28</f>
         <v>IONM</v>
       </c>
       <c r="C11" s="37">
@@ -17056,7 +17336,7 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="str">
-        <f>Commodities!D27</f>
+        <f>Commodities!D29</f>
         <v>IMAP</v>
       </c>
       <c r="C12" s="37">
@@ -17070,7 +17350,7 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="str">
-        <f>Commodities!D28</f>
+        <f>Commodities!D30</f>
         <v>IMAE</v>
       </c>
       <c r="C13" s="37">
@@ -17084,7 +17364,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="str">
-        <f>Commodities!D29</f>
+        <f>Commodities!D31</f>
         <v>IEOE</v>
       </c>
       <c r="C14" s="37">
@@ -17098,7 +17378,7 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="str">
-        <f>Commodities!D30</f>
+        <f>Commodities!D32</f>
         <v>ITEM</v>
       </c>
       <c r="C15" s="37">
@@ -17112,7 +17392,7 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="str">
-        <f>Commodities!D31</f>
+        <f>Commodities!D33</f>
         <v>IOMA</v>
       </c>
       <c r="C16" s="37">
@@ -17126,7 +17406,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="str">
-        <f>Commodities!D32</f>
+        <f>Commodities!D34</f>
         <v>ICON</v>
       </c>
       <c r="C17" s="37">

</xml_diff>